<commit_message>
Update of GINF2 "Professeur"
</commit_message>
<xml_diff>
--- a/resources/GINF2/professeur.xlsx
+++ b/resources/GINF2/professeur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DCC1056-8FBF-495B-8ED2-ACED882B6B28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D894C0C-E9DB-42AE-90A9-A1AC68251EA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
+    <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>CIN</t>
   </si>
@@ -37,6 +37,45 @@
   </si>
   <si>
     <t>DEPARTEMENT</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Badir</t>
+  </si>
+  <si>
+    <t>El Alami</t>
+  </si>
+  <si>
+    <t>Hassoun</t>
+  </si>
+  <si>
+    <t>Amechnoue</t>
+  </si>
+  <si>
+    <t>Khalid</t>
+  </si>
+  <si>
+    <t>Fissoune</t>
+  </si>
+  <si>
+    <t>Rachida</t>
+  </si>
+  <si>
+    <t>Azzouzi</t>
+  </si>
+  <si>
+    <t>Rahali</t>
+  </si>
+  <si>
+    <t>Matières enseignés</t>
   </si>
 </sst>
 </file>
@@ -388,15 +427,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DE032-F837-48F3-9999-072D67E79C55}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,6 +451,57 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Réduction des données à GINF2
</commit_message>
<xml_diff>
--- a/resources/GINF2/professeur.xlsx
+++ b/resources/GINF2/professeur.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\excel_to_xml\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBCE309-87EF-4669-9081-DE5F1DEE915D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD1E23-AC96-4C87-9040-53F8E7212351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
+    <workbookView xWindow="4515" yWindow="2565" windowWidth="15375" windowHeight="8325" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>CIN</t>
-  </si>
-  <si>
-    <t>NOM</t>
-  </si>
-  <si>
-    <t>PRENOM</t>
-  </si>
-  <si>
-    <t>DEPARTEMENT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>El Haddad</t>
   </si>
@@ -69,26 +57,88 @@
     <t>Rachida</t>
   </si>
   <si>
-    <t>Azzouzi</t>
-  </si>
-  <si>
     <t>Rahali</t>
   </si>
   <si>
-    <t>Matières enseignés</t>
+    <t>CNE</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Dept_Attachement</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>El Azzouzi</t>
+  </si>
+  <si>
+    <t>06 82 02 22 11</t>
+  </si>
+  <si>
+    <t>02 51 40 28 06</t>
+  </si>
+  <si>
+    <t>08 55 45 51 46</t>
+  </si>
+  <si>
+    <t>03 42 67 10 87</t>
+  </si>
+  <si>
+    <t>08 89 02 36 34</t>
+  </si>
+  <si>
+    <t>08 44 72 02 14</t>
+  </si>
+  <si>
+    <t>mattis.Integer@tellus.net</t>
+  </si>
+  <si>
+    <t>hendrerit.a.arcu@massanonante.org</t>
+  </si>
+  <si>
+    <t>eros.non.enim@erosturpis.org</t>
+  </si>
+  <si>
+    <t>mauris.sapien.cursus@dolor.net</t>
+  </si>
+  <si>
+    <t>quis.turpis@congue.ca</t>
+  </si>
+  <si>
+    <t>at.fringilla@etcommodoat.net</t>
+  </si>
+  <si>
+    <t>SIC</t>
+  </si>
+  <si>
+    <t>MI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,14 +158,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{24DBDB46-4842-4C17-825C-A7F3B124709C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,82 +481,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DE032-F837-48F3-9999-072D67E79C55}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>